<commit_message>
Several fixes to register
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20160208_1.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20160208_1.xlsx
@@ -2406,7 +2406,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2639,6 +2639,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="27"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3565,7 +3577,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="805">
+  <cellXfs count="808">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4969,9 +4981,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="71" fillId="31" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="71" fillId="31" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="71" fillId="31" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5169,48 +5178,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -5245,6 +5212,9 @@
     <xf numFmtId="3" fontId="11" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5293,17 +5263,122 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="32" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="32" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="32" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="32" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="19" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5317,107 +5392,41 @@
     <xf numFmtId="0" fontId="11" fillId="17" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="19" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="64" fillId="31" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5514,6 +5523,31 @@
     <xf numFmtId="3" fontId="12" fillId="11" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="69" fillId="32" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="69" fillId="39" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5550,31 +5584,12 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="69" fillId="32" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="69" fillId="39" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="71" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="71" fillId="40" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="41" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Hyperlink 2" xfId="10"/>
@@ -5764,7 +5779,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5955,11 +5969,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="311477744"/>
-        <c:axId val="311478304"/>
+        <c:axId val="214729040"/>
+        <c:axId val="211888336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="311477744"/>
+        <c:axId val="214729040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5991,7 +6005,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6058,7 +6071,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311478304"/>
+        <c:crossAx val="211888336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6066,7 +6079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="311478304"/>
+        <c:axId val="211888336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6185,7 +6198,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311477744"/>
+        <c:crossAx val="214729040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6571,11 +6584,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="312973344"/>
-        <c:axId val="312973904"/>
+        <c:axId val="256190256"/>
+        <c:axId val="256190816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="312973344"/>
+        <c:axId val="256190256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6673,7 +6686,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312973904"/>
+        <c:crossAx val="256190816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6681,7 +6694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312973904"/>
+        <c:axId val="256190816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6801,7 +6814,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312973344"/>
+        <c:crossAx val="256190256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7685,11 +7698,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313333792"/>
-        <c:axId val="313334352"/>
+        <c:axId val="257247568"/>
+        <c:axId val="257248128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313333792"/>
+        <c:axId val="257247568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7792,7 +7805,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313334352"/>
+        <c:crossAx val="257248128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7800,7 +7813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313334352"/>
+        <c:axId val="257248128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7851,7 +7864,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313333792"/>
+        <c:crossAx val="257247568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8216,11 +8229,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313337712"/>
-        <c:axId val="313338272"/>
+        <c:axId val="257251488"/>
+        <c:axId val="257252048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313337712"/>
+        <c:axId val="257251488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8331,7 +8344,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313338272"/>
+        <c:crossAx val="257252048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8339,7 +8352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313338272"/>
+        <c:axId val="257252048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8445,7 +8458,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313337712"/>
+        <c:crossAx val="257251488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8815,11 +8828,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="314034656"/>
-        <c:axId val="314035216"/>
+        <c:axId val="251968672"/>
+        <c:axId val="251969232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="314034656"/>
+        <c:axId val="251968672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8930,7 +8943,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314035216"/>
+        <c:crossAx val="251969232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8938,7 +8951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314035216"/>
+        <c:axId val="251969232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9052,7 +9065,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314034656"/>
+        <c:crossAx val="251968672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9187,7 +9200,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9534,11 +9546,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="314040256"/>
-        <c:axId val="314040816"/>
+        <c:axId val="209639616"/>
+        <c:axId val="209640176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="314040256"/>
+        <c:axId val="209639616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9644,7 +9656,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314040816"/>
+        <c:crossAx val="209640176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9652,7 +9664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314040816"/>
+        <c:axId val="209640176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9774,7 +9786,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314040256"/>
+        <c:crossAx val="209639616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10110,11 +10122,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313858192"/>
-        <c:axId val="313858752"/>
+        <c:axId val="209643536"/>
+        <c:axId val="209644096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313858192"/>
+        <c:axId val="209643536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10225,7 +10237,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313858752"/>
+        <c:crossAx val="209644096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10233,7 +10245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313858752"/>
+        <c:axId val="209644096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10347,7 +10359,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313858192"/>
+        <c:crossAx val="209643536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10683,11 +10695,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313862112"/>
-        <c:axId val="313862672"/>
+        <c:axId val="209647456"/>
+        <c:axId val="209648016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313862112"/>
+        <c:axId val="209647456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10798,7 +10810,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313862672"/>
+        <c:crossAx val="209648016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10806,7 +10818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313862672"/>
+        <c:axId val="209648016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10920,7 +10932,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313862112"/>
+        <c:crossAx val="209647456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11301,11 +11313,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="314377376"/>
-        <c:axId val="314377936"/>
+        <c:axId val="209651376"/>
+        <c:axId val="209651936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="314377376"/>
+        <c:axId val="209651376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11403,7 +11415,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314377936"/>
+        <c:crossAx val="209651936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11411,7 +11423,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314377936"/>
+        <c:axId val="209651936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11530,7 +11542,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314377376"/>
+        <c:crossAx val="209651376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11855,11 +11867,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="312580832"/>
-        <c:axId val="312581392"/>
+        <c:axId val="211891696"/>
+        <c:axId val="211892256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="312580832"/>
+        <c:axId val="211891696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11957,7 +11969,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312581392"/>
+        <c:crossAx val="211892256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11965,7 +11977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312581392"/>
+        <c:axId val="211892256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12084,7 +12096,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312580832"/>
+        <c:crossAx val="211891696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12214,7 +12226,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12445,9 +12456,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -13005,11 +13014,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="310747904"/>
-        <c:axId val="310748464"/>
+        <c:axId val="256230096"/>
+        <c:axId val="256230656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="310747904"/>
+        <c:axId val="256230096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13107,7 +13116,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310748464"/>
+        <c:crossAx val="256230656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13115,7 +13124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310748464"/>
+        <c:axId val="256230656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13221,7 +13230,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310747904"/>
+        <c:crossAx val="256230096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13665,11 +13674,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="312551360"/>
-        <c:axId val="312551920"/>
+        <c:axId val="251516896"/>
+        <c:axId val="251517456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="312551360"/>
+        <c:axId val="251516896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13767,7 +13776,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312551920"/>
+        <c:crossAx val="251517456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13775,7 +13784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312551920"/>
+        <c:axId val="251517456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13894,7 +13903,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312551360"/>
+        <c:crossAx val="251516896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14333,11 +14342,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="312762016"/>
-        <c:axId val="312762576"/>
+        <c:axId val="251521376"/>
+        <c:axId val="251521936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="312762016"/>
+        <c:axId val="251521376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14435,7 +14444,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312762576"/>
+        <c:crossAx val="251521936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14443,7 +14452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312762576"/>
+        <c:axId val="251521936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14562,7 +14571,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312762016"/>
+        <c:crossAx val="251521376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15105,11 +15114,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="312768160"/>
-        <c:axId val="312768720"/>
+        <c:axId val="252277872"/>
+        <c:axId val="252278432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="312768160"/>
+        <c:axId val="252277872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15152,7 +15161,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312768720"/>
+        <c:crossAx val="252278432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15160,7 +15169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312768720"/>
+        <c:axId val="252278432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15271,7 +15280,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312768160"/>
+        <c:crossAx val="252277872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15801,11 +15810,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="312944176"/>
-        <c:axId val="312944736"/>
+        <c:axId val="252281792"/>
+        <c:axId val="252282352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="312944176"/>
+        <c:axId val="252281792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15848,7 +15857,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312944736"/>
+        <c:crossAx val="252282352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15856,7 +15865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312944736"/>
+        <c:axId val="252282352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15975,7 +15984,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312944176"/>
+        <c:crossAx val="252281792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16315,11 +16324,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="313307360"/>
-        <c:axId val="313307920"/>
+        <c:axId val="256186336"/>
+        <c:axId val="256186896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="313307360"/>
+        <c:axId val="256186336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16414,7 +16423,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313307920"/>
+        <c:crossAx val="256186896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16422,7 +16431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="313307920"/>
+        <c:axId val="256186896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -16542,7 +16551,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313307360"/>
+        <c:crossAx val="256186336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27443,54 +27452,54 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="663" t="s">
+      <c r="A4" s="662" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="664"/>
-      <c r="C4" s="664"/>
-      <c r="D4" s="664"/>
-      <c r="E4" s="665"/>
-      <c r="F4" s="665"/>
-      <c r="G4" s="665"/>
-      <c r="H4" s="665"/>
-      <c r="I4" s="665"/>
-      <c r="J4" s="665"/>
-      <c r="K4" s="665"/>
-      <c r="L4" s="665"/>
-      <c r="M4" s="665"/>
-      <c r="N4" s="665"/>
-      <c r="O4" s="665"/>
-      <c r="P4" s="665"/>
-      <c r="Q4" s="665"/>
-      <c r="R4" s="665"/>
-      <c r="S4" s="665"/>
-      <c r="T4" s="665"/>
-      <c r="U4" s="665"/>
-      <c r="V4" s="665"/>
-      <c r="W4" s="665"/>
-      <c r="X4" s="665"/>
-      <c r="Y4" s="665"/>
-      <c r="Z4" s="665"/>
-      <c r="AA4" s="665"/>
-      <c r="AB4" s="665"/>
-      <c r="AC4" s="665"/>
-      <c r="AD4" s="665"/>
-      <c r="AE4" s="665"/>
-      <c r="AF4" s="665"/>
-      <c r="AG4" s="665"/>
-      <c r="AH4" s="665"/>
-      <c r="AI4" s="665"/>
-      <c r="AJ4" s="665"/>
-      <c r="AK4" s="665"/>
-      <c r="AL4" s="665"/>
-      <c r="AM4" s="665"/>
-      <c r="AN4" s="665"/>
-      <c r="AO4" s="665"/>
-      <c r="AP4" s="665"/>
-      <c r="AQ4" s="666" t="s">
+      <c r="B4" s="663"/>
+      <c r="C4" s="663"/>
+      <c r="D4" s="663"/>
+      <c r="E4" s="664"/>
+      <c r="F4" s="664"/>
+      <c r="G4" s="664"/>
+      <c r="H4" s="664"/>
+      <c r="I4" s="664"/>
+      <c r="J4" s="664"/>
+      <c r="K4" s="664"/>
+      <c r="L4" s="664"/>
+      <c r="M4" s="664"/>
+      <c r="N4" s="664"/>
+      <c r="O4" s="664"/>
+      <c r="P4" s="664"/>
+      <c r="Q4" s="664"/>
+      <c r="R4" s="664"/>
+      <c r="S4" s="664"/>
+      <c r="T4" s="664"/>
+      <c r="U4" s="664"/>
+      <c r="V4" s="664"/>
+      <c r="W4" s="664"/>
+      <c r="X4" s="664"/>
+      <c r="Y4" s="664"/>
+      <c r="Z4" s="664"/>
+      <c r="AA4" s="664"/>
+      <c r="AB4" s="664"/>
+      <c r="AC4" s="664"/>
+      <c r="AD4" s="664"/>
+      <c r="AE4" s="664"/>
+      <c r="AF4" s="664"/>
+      <c r="AG4" s="664"/>
+      <c r="AH4" s="664"/>
+      <c r="AI4" s="664"/>
+      <c r="AJ4" s="664"/>
+      <c r="AK4" s="664"/>
+      <c r="AL4" s="664"/>
+      <c r="AM4" s="664"/>
+      <c r="AN4" s="664"/>
+      <c r="AO4" s="664"/>
+      <c r="AP4" s="664"/>
+      <c r="AQ4" s="665" t="s">
         <v>3</v>
       </c>
-      <c r="AR4" s="666"/>
+      <c r="AR4" s="665"/>
     </row>
     <row r="5" spans="1:44" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="414" t="s">
@@ -27786,7 +27795,7 @@
       <c r="B21" s="395" t="s">
         <v>326</v>
       </c>
-      <c r="C21" s="636"/>
+      <c r="C21" s="635"/>
     </row>
     <row r="22" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="394" t="s">
@@ -27795,7 +27804,7 @@
       <c r="B22" s="395" t="s">
         <v>328</v>
       </c>
-      <c r="C22" s="635"/>
+      <c r="C22" s="634"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="383" t="s">
@@ -27864,20 +27873,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="790" t="s">
+      <c r="A3" s="798" t="s">
         <v>347</v>
       </c>
-      <c r="B3" s="792" t="s">
+      <c r="B3" s="800" t="s">
         <v>348</v>
       </c>
-      <c r="C3" s="793"/>
-      <c r="D3" s="788" t="s">
+      <c r="C3" s="801"/>
+      <c r="D3" s="796" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="789"/>
+      <c r="E3" s="797"/>
     </row>
     <row r="4" spans="1:28" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="791"/>
+      <c r="A4" s="799"/>
       <c r="B4" s="427" t="s">
         <v>224</v>
       </c>
@@ -28000,7 +28009,7 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="790" t="s">
+      <c r="A13" s="798" t="s">
         <v>351</v>
       </c>
       <c r="B13" s="426" t="s">
@@ -28023,7 +28032,7 @@
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="791"/>
+      <c r="A14" s="799"/>
       <c r="B14" s="429" t="s">
         <v>352</v>
       </c>
@@ -28082,14 +28091,14 @@
       <c r="A22" s="431" t="s">
         <v>311</v>
       </c>
-      <c r="B22" s="794" t="s">
+      <c r="B22" s="802" t="s">
         <v>348</v>
       </c>
-      <c r="C22" s="795"/>
-      <c r="D22" s="794" t="s">
+      <c r="C22" s="803"/>
+      <c r="D22" s="802" t="s">
         <v>462</v>
       </c>
-      <c r="E22" s="795"/>
+      <c r="E22" s="803"/>
     </row>
     <row r="23" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="432"/>
@@ -28123,9 +28132,9 @@
         <v>314</v>
       </c>
       <c r="B24" s="504"/>
-      <c r="C24" s="658"/>
+      <c r="C24" s="657"/>
       <c r="D24" s="435"/>
-      <c r="E24" s="641"/>
+      <c r="E24" s="640"/>
       <c r="Z24" t="str">
         <f t="shared" ref="Z24:Z29" si="1">A25</f>
         <v xml:space="preserve">re-used: Soil and agriculture </v>
@@ -28148,9 +28157,9 @@
         <v>359</v>
       </c>
       <c r="B25" s="515"/>
-      <c r="C25" s="659"/>
+      <c r="C25" s="658"/>
       <c r="D25" s="435"/>
-      <c r="E25" s="641"/>
+      <c r="E25" s="640"/>
       <c r="Z25" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">re-used: Others </v>
@@ -28173,9 +28182,9 @@
         <v>360</v>
       </c>
       <c r="B26" s="506"/>
-      <c r="C26" s="660"/>
+      <c r="C26" s="659"/>
       <c r="D26" s="435"/>
-      <c r="E26" s="641"/>
+      <c r="E26" s="640"/>
       <c r="Z26" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">disposed: Landfill </v>
@@ -28198,9 +28207,9 @@
         <v>454</v>
       </c>
       <c r="B27" s="506"/>
-      <c r="C27" s="660"/>
+      <c r="C27" s="659"/>
       <c r="D27" s="435"/>
-      <c r="E27" s="641"/>
+      <c r="E27" s="640"/>
       <c r="Z27" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">disposed: Incineration </v>
@@ -28223,9 +28232,9 @@
         <v>361</v>
       </c>
       <c r="B28" s="506"/>
-      <c r="C28" s="660"/>
+      <c r="C28" s="659"/>
       <c r="D28" s="435"/>
-      <c r="E28" s="641"/>
+      <c r="E28" s="640"/>
       <c r="Z28" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">disposed: Others </v>
@@ -28248,9 +28257,9 @@
         <v>362</v>
       </c>
       <c r="B29" s="506"/>
-      <c r="C29" s="660"/>
+      <c r="C29" s="659"/>
       <c r="D29" s="435"/>
-      <c r="E29" s="641"/>
+      <c r="E29" s="640"/>
       <c r="Z29" t="str">
         <f t="shared" si="1"/>
         <v>Other</v>
@@ -28273,9 +28282,9 @@
         <v>461</v>
       </c>
       <c r="B30" s="506"/>
-      <c r="C30" s="660"/>
+      <c r="C30" s="659"/>
       <c r="D30" s="435"/>
-      <c r="E30" s="641"/>
+      <c r="E30" s="640"/>
     </row>
     <row r="35" spans="1:32" ht="33" x14ac:dyDescent="0.35">
       <c r="A35" s="436" t="s">
@@ -28298,8 +28307,8 @@
       <c r="B36" s="439" t="s">
         <v>326</v>
       </c>
-      <c r="C36" s="637"/>
-      <c r="D36" s="637"/>
+      <c r="C36" s="636"/>
+      <c r="D36" s="636"/>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="438" t="s">
@@ -28308,21 +28317,21 @@
       <c r="B37" s="439" t="s">
         <v>328</v>
       </c>
-      <c r="C37" s="657"/>
-      <c r="D37" s="657"/>
+      <c r="C37" s="656"/>
+      <c r="D37" s="656"/>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="434" t="s">
         <v>363</v>
       </c>
-      <c r="B41" s="784" t="s">
+      <c r="B41" s="792" t="s">
         <v>348</v>
       </c>
-      <c r="C41" s="785"/>
-      <c r="D41" s="786" t="s">
+      <c r="C41" s="793"/>
+      <c r="D41" s="794" t="s">
         <v>357</v>
       </c>
-      <c r="E41" s="787"/>
+      <c r="E41" s="795"/>
       <c r="AA41" t="s">
         <v>439</v>
       </c>
@@ -28994,14 +29003,14 @@
       <c r="A77" s="458" t="s">
         <v>269</v>
       </c>
-      <c r="B77" s="638"/>
-      <c r="C77" s="646"/>
-      <c r="D77" s="638"/>
-      <c r="E77" s="646"/>
+      <c r="B77" s="637"/>
+      <c r="C77" s="645"/>
+      <c r="D77" s="637"/>
+      <c r="E77" s="645"/>
       <c r="F77" s="489"/>
-      <c r="G77" s="649"/>
+      <c r="G77" s="648"/>
       <c r="H77" s="490"/>
-      <c r="I77" s="653"/>
+      <c r="I77" s="652"/>
       <c r="Z77" t="s">
         <v>269</v>
       </c>
@@ -29030,13 +29039,13 @@
         <v>258</v>
       </c>
       <c r="B78" s="491"/>
-      <c r="C78" s="647"/>
+      <c r="C78" s="646"/>
       <c r="D78" s="492"/>
-      <c r="E78" s="647"/>
+      <c r="E78" s="646"/>
       <c r="F78" s="491"/>
-      <c r="G78" s="650"/>
+      <c r="G78" s="649"/>
       <c r="H78" s="492"/>
-      <c r="I78" s="654"/>
+      <c r="I78" s="653"/>
       <c r="Z78" s="238" t="s">
         <v>258</v>
       </c>
@@ -29065,13 +29074,13 @@
         <v>386</v>
       </c>
       <c r="B79" s="491"/>
-      <c r="C79" s="647"/>
+      <c r="C79" s="646"/>
       <c r="D79" s="492"/>
-      <c r="E79" s="647"/>
+      <c r="E79" s="646"/>
       <c r="F79" s="491"/>
-      <c r="G79" s="650"/>
+      <c r="G79" s="649"/>
       <c r="H79" s="492"/>
-      <c r="I79" s="654"/>
+      <c r="I79" s="653"/>
       <c r="Z79" s="238" t="s">
         <v>386</v>
       </c>
@@ -29100,13 +29109,13 @@
         <v>387</v>
       </c>
       <c r="B80" s="491"/>
-      <c r="C80" s="647"/>
+      <c r="C80" s="646"/>
       <c r="D80" s="492"/>
-      <c r="E80" s="647"/>
+      <c r="E80" s="646"/>
       <c r="F80" s="491"/>
-      <c r="G80" s="650"/>
+      <c r="G80" s="649"/>
       <c r="H80" s="492"/>
-      <c r="I80" s="654"/>
+      <c r="I80" s="653"/>
       <c r="Z80" s="238" t="s">
         <v>387</v>
       </c>
@@ -29135,13 +29144,13 @@
         <v>388</v>
       </c>
       <c r="B81" s="493"/>
-      <c r="C81" s="647"/>
+      <c r="C81" s="646"/>
       <c r="D81" s="494"/>
-      <c r="E81" s="647"/>
+      <c r="E81" s="646"/>
       <c r="F81" s="493"/>
-      <c r="G81" s="651"/>
+      <c r="G81" s="650"/>
       <c r="H81" s="494"/>
-      <c r="I81" s="655"/>
+      <c r="I81" s="654"/>
       <c r="Z81" s="238" t="s">
         <v>388</v>
       </c>
@@ -29170,13 +29179,13 @@
         <v>389</v>
       </c>
       <c r="B82" s="495"/>
-      <c r="C82" s="648"/>
+      <c r="C82" s="647"/>
       <c r="D82" s="496"/>
-      <c r="E82" s="648"/>
+      <c r="E82" s="647"/>
       <c r="F82" s="495"/>
-      <c r="G82" s="652"/>
+      <c r="G82" s="651"/>
       <c r="H82" s="496"/>
-      <c r="I82" s="656"/>
+      <c r="I82" s="655"/>
       <c r="Z82" s="459" t="s">
         <v>389</v>
       </c>
@@ -29206,14 +29215,14 @@
       </c>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B85" s="798" t="s">
+      <c r="B85" s="785" t="s">
         <v>348</v>
       </c>
-      <c r="C85" s="799"/>
-      <c r="D85" s="798" t="s">
+      <c r="C85" s="786"/>
+      <c r="D85" s="785" t="s">
         <v>357</v>
       </c>
-      <c r="E85" s="799"/>
+      <c r="E85" s="786"/>
       <c r="Z85" t="s">
         <v>453</v>
       </c>
@@ -29226,14 +29235,14 @@
     </row>
     <row r="86" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="299"/>
-      <c r="B86" s="800" t="s">
+      <c r="B86" s="787" t="s">
         <v>256</v>
       </c>
-      <c r="C86" s="753"/>
-      <c r="D86" s="800" t="s">
+      <c r="C86" s="752"/>
+      <c r="D86" s="787" t="s">
         <v>256</v>
       </c>
-      <c r="E86" s="753"/>
+      <c r="E86" s="752"/>
       <c r="Z86" s="461" t="s">
         <v>257</v>
       </c>
@@ -29278,11 +29287,11 @@
       <c r="A88" s="461" t="s">
         <v>257</v>
       </c>
-      <c r="B88" s="643">
+      <c r="B88" s="642">
         <v>100</v>
       </c>
       <c r="C88" s="498"/>
-      <c r="D88" s="643">
+      <c r="D88" s="642">
         <v>100</v>
       </c>
       <c r="E88" s="498"/>
@@ -29302,9 +29311,9 @@
       <c r="A89" s="462" t="s">
         <v>391</v>
       </c>
-      <c r="B89" s="643"/>
+      <c r="B89" s="642"/>
       <c r="C89" s="435"/>
-      <c r="D89" s="643"/>
+      <c r="D89" s="642"/>
       <c r="E89" s="435"/>
       <c r="Z89" s="462" t="s">
         <v>393</v>
@@ -29322,11 +29331,11 @@
       <c r="A90" s="461" t="s">
         <v>392</v>
       </c>
-      <c r="B90" s="643">
+      <c r="B90" s="642">
         <v>100</v>
       </c>
       <c r="C90" s="498"/>
-      <c r="D90" s="643">
+      <c r="D90" s="642">
         <v>100</v>
       </c>
       <c r="E90" s="498"/>
@@ -29346,9 +29355,9 @@
       <c r="A91" s="462" t="s">
         <v>393</v>
       </c>
-      <c r="B91" s="644"/>
+      <c r="B91" s="643"/>
       <c r="C91" s="435"/>
-      <c r="D91" s="644"/>
+      <c r="D91" s="643"/>
       <c r="E91" s="435"/>
       <c r="Z91" s="463" t="s">
         <v>395</v>
@@ -29366,9 +29375,9 @@
       <c r="A92" s="462" t="s">
         <v>394</v>
       </c>
-      <c r="B92" s="644"/>
+      <c r="B92" s="643"/>
       <c r="C92" s="435"/>
-      <c r="D92" s="644"/>
+      <c r="D92" s="643"/>
       <c r="E92" s="435"/>
       <c r="Z92" s="462" t="s">
         <v>396</v>
@@ -29386,11 +29395,11 @@
       <c r="A93" s="463" t="s">
         <v>395</v>
       </c>
-      <c r="B93" s="645">
+      <c r="B93" s="644">
         <v>100</v>
       </c>
       <c r="C93" s="498"/>
-      <c r="D93" s="645">
+      <c r="D93" s="644">
         <v>100</v>
       </c>
       <c r="E93" s="498">
@@ -29412,25 +29421,25 @@
       <c r="A94" s="462" t="s">
         <v>396</v>
       </c>
-      <c r="B94" s="644"/>
+      <c r="B94" s="643"/>
       <c r="C94" s="435"/>
-      <c r="D94" s="644"/>
+      <c r="D94" s="643"/>
       <c r="E94" s="435"/>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" s="462" t="s">
         <v>397</v>
       </c>
-      <c r="B95" s="644"/>
+      <c r="B95" s="643"/>
       <c r="C95" s="435"/>
-      <c r="D95" s="644"/>
+      <c r="D95" s="643"/>
       <c r="E95" s="435"/>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" s="464"/>
-      <c r="B96" s="641"/>
+      <c r="B96" s="640"/>
       <c r="C96" s="435"/>
-      <c r="D96" s="641"/>
+      <c r="D96" s="640"/>
       <c r="E96" s="435"/>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.25">
@@ -29439,25 +29448,25 @@
       </c>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B101" s="798" t="s">
+      <c r="B101" s="785" t="s">
         <v>348</v>
       </c>
-      <c r="C101" s="799"/>
-      <c r="D101" s="798" t="s">
+      <c r="C101" s="786"/>
+      <c r="D101" s="785" t="s">
         <v>357</v>
       </c>
-      <c r="E101" s="799"/>
+      <c r="E101" s="786"/>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102" s="299"/>
-      <c r="B102" s="800" t="s">
+      <c r="B102" s="787" t="s">
         <v>256</v>
       </c>
-      <c r="C102" s="753"/>
-      <c r="D102" s="800" t="s">
+      <c r="C102" s="752"/>
+      <c r="D102" s="787" t="s">
         <v>256</v>
       </c>
-      <c r="E102" s="753"/>
+      <c r="E102" s="752"/>
       <c r="Z102" t="s">
         <v>453</v>
       </c>
@@ -29500,11 +29509,11 @@
       <c r="A104" s="461" t="s">
         <v>257</v>
       </c>
-      <c r="B104" s="643">
+      <c r="B104" s="642">
         <v>100</v>
       </c>
       <c r="C104" s="498"/>
-      <c r="D104" s="643">
+      <c r="D104" s="642">
         <v>100</v>
       </c>
       <c r="E104" s="498"/>
@@ -29524,9 +29533,9 @@
       <c r="A105" s="462" t="s">
         <v>391</v>
       </c>
-      <c r="B105" s="643"/>
+      <c r="B105" s="642"/>
       <c r="C105" s="435"/>
-      <c r="D105" s="643"/>
+      <c r="D105" s="642"/>
       <c r="E105" s="435"/>
       <c r="Z105" s="461" t="s">
         <v>392</v>
@@ -29544,11 +29553,11 @@
       <c r="A106" s="461" t="s">
         <v>392</v>
       </c>
-      <c r="B106" s="643">
+      <c r="B106" s="642">
         <v>100</v>
       </c>
       <c r="C106" s="498"/>
-      <c r="D106" s="643">
+      <c r="D106" s="642">
         <v>100</v>
       </c>
       <c r="E106" s="498"/>
@@ -29568,9 +29577,9 @@
       <c r="A107" s="462" t="s">
         <v>393</v>
       </c>
-      <c r="B107" s="644"/>
+      <c r="B107" s="643"/>
       <c r="C107" s="435"/>
-      <c r="D107" s="644"/>
+      <c r="D107" s="643"/>
       <c r="E107" s="435"/>
       <c r="Z107" s="462" t="s">
         <v>394</v>
@@ -29588,9 +29597,9 @@
       <c r="A108" s="462" t="s">
         <v>394</v>
       </c>
-      <c r="B108" s="644"/>
+      <c r="B108" s="643"/>
       <c r="C108" s="435"/>
-      <c r="D108" s="644"/>
+      <c r="D108" s="643"/>
       <c r="E108" s="435"/>
       <c r="Z108" s="463" t="s">
         <v>395</v>
@@ -29608,11 +29617,11 @@
       <c r="A109" s="463" t="s">
         <v>395</v>
       </c>
-      <c r="B109" s="645">
+      <c r="B109" s="644">
         <v>100</v>
       </c>
       <c r="C109" s="498"/>
-      <c r="D109" s="645">
+      <c r="D109" s="644">
         <v>100</v>
       </c>
       <c r="E109" s="498"/>
@@ -29632,9 +29641,9 @@
       <c r="A110" s="462" t="s">
         <v>396</v>
       </c>
-      <c r="B110" s="644"/>
+      <c r="B110" s="643"/>
       <c r="C110" s="435"/>
-      <c r="D110" s="644"/>
+      <c r="D110" s="643"/>
       <c r="E110" s="435"/>
       <c r="Z110" s="462" t="s">
         <v>397</v>
@@ -29652,16 +29661,16 @@
       <c r="A111" s="462" t="s">
         <v>397</v>
       </c>
-      <c r="B111" s="644"/>
+      <c r="B111" s="643"/>
       <c r="C111" s="435"/>
-      <c r="D111" s="644"/>
+      <c r="D111" s="643"/>
       <c r="E111" s="435"/>
     </row>
     <row r="112" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A112" s="464"/>
-      <c r="B112" s="641"/>
+      <c r="B112" s="640"/>
       <c r="C112" s="435"/>
-      <c r="D112" s="641"/>
+      <c r="D112" s="640"/>
       <c r="E112" s="435"/>
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.25">
@@ -29670,25 +29679,25 @@
       </c>
     </row>
     <row r="116" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B116" s="801" t="s">
+      <c r="B116" s="788" t="s">
         <v>348</v>
       </c>
-      <c r="C116" s="802"/>
-      <c r="D116" s="801" t="s">
+      <c r="C116" s="789"/>
+      <c r="D116" s="788" t="s">
         <v>357</v>
       </c>
-      <c r="E116" s="802"/>
+      <c r="E116" s="789"/>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" s="466"/>
-      <c r="B117" s="803" t="s">
+      <c r="B117" s="790" t="s">
         <v>256</v>
       </c>
-      <c r="C117" s="804"/>
-      <c r="D117" s="803" t="s">
+      <c r="C117" s="791"/>
+      <c r="D117" s="790" t="s">
         <v>256</v>
       </c>
-      <c r="E117" s="804"/>
+      <c r="E117" s="791"/>
       <c r="Z117" t="s">
         <v>453</v>
       </c>
@@ -29732,11 +29741,11 @@
       <c r="A119" s="461" t="s">
         <v>257</v>
       </c>
-      <c r="B119" s="643">
+      <c r="B119" s="642">
         <v>100</v>
       </c>
       <c r="C119" s="498"/>
-      <c r="D119" s="643">
+      <c r="D119" s="642">
         <v>100</v>
       </c>
       <c r="E119" s="498"/>
@@ -29757,9 +29766,9 @@
       <c r="A120" s="462" t="s">
         <v>391</v>
       </c>
-      <c r="B120" s="643"/>
+      <c r="B120" s="642"/>
       <c r="C120" s="435"/>
-      <c r="D120" s="643"/>
+      <c r="D120" s="642"/>
       <c r="E120" s="435"/>
       <c r="I120" s="499"/>
       <c r="Z120" s="461" t="s">
@@ -29778,11 +29787,11 @@
       <c r="A121" s="461" t="s">
         <v>392</v>
       </c>
-      <c r="B121" s="643">
+      <c r="B121" s="642">
         <v>100</v>
       </c>
       <c r="C121" s="498"/>
-      <c r="D121" s="643">
+      <c r="D121" s="642">
         <v>100</v>
       </c>
       <c r="E121" s="498"/>
@@ -29803,9 +29812,9 @@
       <c r="A122" s="462" t="s">
         <v>393</v>
       </c>
-      <c r="B122" s="644"/>
+      <c r="B122" s="643"/>
       <c r="C122" s="435"/>
-      <c r="D122" s="644"/>
+      <c r="D122" s="643"/>
       <c r="E122" s="435"/>
       <c r="I122" s="499"/>
       <c r="Z122" s="462" t="s">
@@ -29824,9 +29833,9 @@
       <c r="A123" s="462" t="s">
         <v>394</v>
       </c>
-      <c r="B123" s="644"/>
+      <c r="B123" s="643"/>
       <c r="C123" s="435"/>
-      <c r="D123" s="644"/>
+      <c r="D123" s="643"/>
       <c r="E123" s="435"/>
       <c r="I123" s="499"/>
       <c r="Z123" s="463" t="s">
@@ -29845,11 +29854,11 @@
       <c r="A124" s="463" t="s">
         <v>395</v>
       </c>
-      <c r="B124" s="645">
+      <c r="B124" s="644">
         <v>100</v>
       </c>
       <c r="C124" s="498"/>
-      <c r="D124" s="645">
+      <c r="D124" s="644">
         <v>100</v>
       </c>
       <c r="E124" s="498"/>
@@ -29870,9 +29879,9 @@
       <c r="A125" s="462" t="s">
         <v>396</v>
       </c>
-      <c r="B125" s="644"/>
+      <c r="B125" s="643"/>
       <c r="C125" s="435"/>
-      <c r="D125" s="644"/>
+      <c r="D125" s="643"/>
       <c r="E125" s="435"/>
       <c r="I125" s="499"/>
       <c r="Z125" s="462" t="s">
@@ -29891,27 +29900,27 @@
       <c r="A126" s="462" t="s">
         <v>397</v>
       </c>
-      <c r="B126" s="644"/>
+      <c r="B126" s="643"/>
       <c r="C126" s="435"/>
-      <c r="D126" s="644"/>
+      <c r="D126" s="643"/>
       <c r="E126" s="435"/>
     </row>
     <row r="127" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A127" s="464"/>
-      <c r="B127" s="641"/>
+      <c r="B127" s="640"/>
       <c r="C127" s="435"/>
-      <c r="D127" s="641"/>
+      <c r="D127" s="640"/>
       <c r="E127" s="435"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="470" t="s">
         <v>351</v>
       </c>
-      <c r="B129" s="796" t="s">
+      <c r="B129" s="783" t="s">
         <v>348</v>
       </c>
-      <c r="C129" s="797"/>
-      <c r="D129" s="797"/>
+      <c r="C129" s="784"/>
+      <c r="D129" s="784"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="471"/>
@@ -29929,17 +29938,17 @@
       <c r="A131" s="474" t="s">
         <v>400</v>
       </c>
-      <c r="B131" s="641">
+      <c r="B131" s="640">
         <v>100</v>
       </c>
       <c r="C131" s="498"/>
-      <c r="D131" s="639"/>
+      <c r="D131" s="638"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="428" t="s">
         <v>401</v>
       </c>
-      <c r="B132" s="641"/>
+      <c r="B132" s="640"/>
       <c r="C132" s="435"/>
       <c r="D132" s="522"/>
     </row>
@@ -29947,7 +29956,7 @@
       <c r="A133" s="428" t="s">
         <v>259</v>
       </c>
-      <c r="B133" s="641"/>
+      <c r="B133" s="640"/>
       <c r="C133" s="435"/>
       <c r="D133" s="522"/>
     </row>
@@ -29955,7 +29964,7 @@
       <c r="A134" s="428" t="s">
         <v>402</v>
       </c>
-      <c r="B134" s="641"/>
+      <c r="B134" s="640"/>
       <c r="C134" s="435"/>
       <c r="D134" s="522"/>
     </row>
@@ -29963,7 +29972,7 @@
       <c r="A135" s="428" t="s">
         <v>403</v>
       </c>
-      <c r="B135" s="641"/>
+      <c r="B135" s="640"/>
       <c r="C135" s="435"/>
       <c r="D135" s="522"/>
     </row>
@@ -29971,7 +29980,7 @@
       <c r="A136" s="428" t="s">
         <v>404</v>
       </c>
-      <c r="B136" s="641"/>
+      <c r="B136" s="640"/>
       <c r="C136" s="435"/>
       <c r="D136" s="522"/>
     </row>
@@ -29979,7 +29988,7 @@
       <c r="A137" s="428" t="s">
         <v>405</v>
       </c>
-      <c r="B137" s="641"/>
+      <c r="B137" s="640"/>
       <c r="C137" s="435"/>
       <c r="D137" s="522"/>
     </row>
@@ -29987,7 +29996,7 @@
       <c r="A138" s="428" t="s">
         <v>406</v>
       </c>
-      <c r="B138" s="641"/>
+      <c r="B138" s="640"/>
       <c r="C138" s="435"/>
       <c r="D138" s="522"/>
     </row>
@@ -29995,7 +30004,7 @@
       <c r="A139" s="428" t="s">
         <v>407</v>
       </c>
-      <c r="B139" s="641"/>
+      <c r="B139" s="640"/>
       <c r="C139" s="435"/>
       <c r="D139" s="522"/>
     </row>
@@ -30032,7 +30041,7 @@
         <v>132</v>
       </c>
       <c r="C148" s="435"/>
-      <c r="D148" s="640"/>
+      <c r="D148" s="639"/>
       <c r="Z148" s="480" t="s">
         <v>409</v>
       </c>
@@ -30050,7 +30059,7 @@
         <v>132</v>
       </c>
       <c r="C149" s="435"/>
-      <c r="D149" s="640"/>
+      <c r="D149" s="639"/>
       <c r="Z149" s="480" t="s">
         <v>411</v>
       </c>
@@ -30068,7 +30077,7 @@
         <v>132</v>
       </c>
       <c r="C150" s="435"/>
-      <c r="D150" s="640"/>
+      <c r="D150" s="639"/>
       <c r="Z150" s="480" t="s">
         <v>413</v>
       </c>
@@ -30086,7 +30095,7 @@
         <v>132</v>
       </c>
       <c r="C151" s="435"/>
-      <c r="D151" s="640"/>
+      <c r="D151" s="639"/>
       <c r="Z151" s="480" t="s">
         <v>415</v>
       </c>
@@ -30104,7 +30113,7 @@
         <v>132</v>
       </c>
       <c r="C152" s="435"/>
-      <c r="D152" s="640"/>
+      <c r="D152" s="639"/>
     </row>
     <row r="153" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A153" s="480" t="s">
@@ -30114,7 +30123,7 @@
         <v>132</v>
       </c>
       <c r="C153" s="435"/>
-      <c r="D153" s="640"/>
+      <c r="D153" s="639"/>
       <c r="Z153" s="476" t="s">
         <v>408</v>
       </c>
@@ -30134,7 +30143,7 @@
         <v>132</v>
       </c>
       <c r="C154" s="435"/>
-      <c r="D154" s="640"/>
+      <c r="D154" s="639"/>
       <c r="Z154" s="480" t="s">
         <v>410</v>
       </c>
@@ -30152,7 +30161,7 @@
         <v>132</v>
       </c>
       <c r="C155" s="435"/>
-      <c r="D155" s="640"/>
+      <c r="D155" s="639"/>
       <c r="Z155" s="480" t="s">
         <v>412</v>
       </c>
@@ -30203,8 +30212,8 @@
       <c r="B159" s="480" t="s">
         <v>127</v>
       </c>
-      <c r="C159" s="641"/>
-      <c r="D159" s="642"/>
+      <c r="C159" s="640"/>
+      <c r="D159" s="641"/>
       <c r="Z159" s="476" t="s">
         <v>408</v>
       </c>
@@ -30223,8 +30232,8 @@
       <c r="B160" s="480" t="s">
         <v>127</v>
       </c>
-      <c r="C160" s="641"/>
-      <c r="D160" s="642"/>
+      <c r="C160" s="640"/>
+      <c r="D160" s="641"/>
       <c r="Z160" s="480" t="s">
         <v>105</v>
       </c>
@@ -30247,8 +30256,8 @@
       <c r="B161" s="480" t="s">
         <v>127</v>
       </c>
-      <c r="C161" s="641"/>
-      <c r="D161" s="642"/>
+      <c r="C161" s="640"/>
+      <c r="D161" s="641"/>
       <c r="Z161" s="480" t="s">
         <v>110</v>
       </c>
@@ -30271,8 +30280,8 @@
       <c r="B162" s="480" t="s">
         <v>127</v>
       </c>
-      <c r="C162" s="641"/>
-      <c r="D162" s="642"/>
+      <c r="C162" s="640"/>
+      <c r="D162" s="641"/>
       <c r="Z162" s="480" t="s">
         <v>115</v>
       </c>
@@ -30328,7 +30337,7 @@
         <v>131</v>
       </c>
       <c r="C166" s="435"/>
-      <c r="D166" s="640"/>
+      <c r="D166" s="639"/>
     </row>
     <row r="168" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A168" s="476" t="s">
@@ -30359,8 +30368,8 @@
       <c r="B169" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C169" s="641"/>
-      <c r="D169" s="642"/>
+      <c r="C169" s="640"/>
+      <c r="D169" s="641"/>
       <c r="Z169" s="480" t="s">
         <v>418</v>
       </c>
@@ -30383,8 +30392,8 @@
       <c r="B170" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C170" s="641"/>
-      <c r="D170" s="642"/>
+      <c r="C170" s="640"/>
+      <c r="D170" s="641"/>
       <c r="Z170" s="480" t="s">
         <v>420</v>
       </c>
@@ -30407,8 +30416,8 @@
       <c r="B171" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C171" s="641"/>
-      <c r="D171" s="642"/>
+      <c r="C171" s="640"/>
+      <c r="D171" s="641"/>
       <c r="Z171" s="480" t="s">
         <v>422</v>
       </c>
@@ -30431,8 +30440,8 @@
       <c r="B172" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C172" s="641"/>
-      <c r="D172" s="642"/>
+      <c r="C172" s="640"/>
+      <c r="D172" s="641"/>
       <c r="Z172" s="480" t="s">
         <v>424</v>
       </c>
@@ -30455,8 +30464,8 @@
       <c r="B173" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C173" s="641"/>
-      <c r="D173" s="642"/>
+      <c r="C173" s="640"/>
+      <c r="D173" s="641"/>
     </row>
     <row r="174" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A174" s="480" t="s">
@@ -30465,8 +30474,8 @@
       <c r="B174" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C174" s="641"/>
-      <c r="D174" s="642"/>
+      <c r="C174" s="640"/>
+      <c r="D174" s="641"/>
       <c r="Z174" s="476" t="s">
         <v>408</v>
       </c>
@@ -30485,8 +30494,8 @@
       <c r="B175" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C175" s="641"/>
-      <c r="D175" s="642"/>
+      <c r="C175" s="640"/>
+      <c r="D175" s="641"/>
       <c r="Z175" s="480" t="s">
         <v>419</v>
       </c>
@@ -30509,8 +30518,8 @@
       <c r="B176" s="480" t="s">
         <v>133</v>
       </c>
-      <c r="C176" s="641"/>
-      <c r="D176" s="642"/>
+      <c r="C176" s="640"/>
+      <c r="D176" s="641"/>
       <c r="Z176" s="480" t="s">
         <v>421</v>
       </c>
@@ -30560,6 +30569,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -30573,14 +30590,6 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
@@ -30687,7 +30696,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="410"/>
       <c r="B6" s="411"/>
-      <c r="C6" s="661"/>
+      <c r="C6" s="660"/>
       <c r="D6" s="412"/>
     </row>
   </sheetData>
@@ -30746,7 +30755,7 @@
       <c r="B5" s="413"/>
       <c r="C5" s="413"/>
       <c r="D5" s="413"/>
-      <c r="E5" s="662"/>
+      <c r="E5" s="661"/>
       <c r="F5" s="412"/>
     </row>
   </sheetData>
@@ -30811,7 +30820,7 @@
       <c r="B6" s="411"/>
       <c r="C6" s="411"/>
       <c r="D6" s="411"/>
-      <c r="E6" s="661"/>
+      <c r="E6" s="660"/>
       <c r="F6" s="412"/>
     </row>
   </sheetData>
@@ -30836,123 +30845,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="667" t="s">
+      <c r="A1" s="695" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="668"/>
-      <c r="C1" s="668"/>
-      <c r="D1" s="668"/>
-      <c r="E1" s="668"/>
-      <c r="F1" s="668"/>
-      <c r="G1" s="668"/>
-      <c r="H1" s="669" t="s">
+      <c r="B1" s="696"/>
+      <c r="C1" s="696"/>
+      <c r="D1" s="696"/>
+      <c r="E1" s="696"/>
+      <c r="F1" s="696"/>
+      <c r="G1" s="696"/>
+      <c r="H1" s="697" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="670"/>
-      <c r="J1" s="670"/>
-      <c r="K1" s="670"/>
-      <c r="L1" s="670"/>
-      <c r="M1" s="671"/>
-      <c r="N1" s="672" t="s">
+      <c r="I1" s="698"/>
+      <c r="J1" s="698"/>
+      <c r="K1" s="698"/>
+      <c r="L1" s="698"/>
+      <c r="M1" s="699"/>
+      <c r="N1" s="700" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="673"/>
-      <c r="P1" s="673"/>
-      <c r="Q1" s="674"/>
-      <c r="R1" s="674"/>
-      <c r="S1" s="673"/>
-      <c r="T1" s="673"/>
-      <c r="U1" s="673"/>
-      <c r="V1" s="675" t="s">
+      <c r="O1" s="678"/>
+      <c r="P1" s="678"/>
+      <c r="Q1" s="701"/>
+      <c r="R1" s="701"/>
+      <c r="S1" s="678"/>
+      <c r="T1" s="678"/>
+      <c r="U1" s="678"/>
+      <c r="V1" s="702" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="676"/>
-      <c r="X1" s="677"/>
-      <c r="Y1" s="677"/>
-      <c r="Z1" s="678"/>
-      <c r="AA1" s="679" t="s">
+      <c r="W1" s="703"/>
+      <c r="X1" s="704"/>
+      <c r="Y1" s="704"/>
+      <c r="Z1" s="705"/>
+      <c r="AA1" s="706" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="680"/>
-      <c r="AC1" s="680"/>
-      <c r="AD1" s="680"/>
-      <c r="AE1" s="680"/>
-      <c r="AF1" s="680"/>
-      <c r="AG1" s="680"/>
-      <c r="AH1" s="680"/>
-      <c r="AI1" s="680"/>
-      <c r="AJ1" s="680"/>
-      <c r="AK1" s="680"/>
-      <c r="AL1" s="680"/>
-      <c r="AM1" s="680"/>
+      <c r="AB1" s="707"/>
+      <c r="AC1" s="707"/>
+      <c r="AD1" s="707"/>
+      <c r="AE1" s="707"/>
+      <c r="AF1" s="707"/>
+      <c r="AG1" s="707"/>
+      <c r="AH1" s="707"/>
+      <c r="AI1" s="707"/>
+      <c r="AJ1" s="707"/>
+      <c r="AK1" s="707"/>
+      <c r="AL1" s="707"/>
+      <c r="AM1" s="707"/>
       <c r="AN1" s="7"/>
       <c r="AO1" s="8"/>
-      <c r="AP1" s="692" t="s">
+      <c r="AP1" s="677" t="s">
         <v>53</v>
       </c>
-      <c r="AQ1" s="673"/>
-      <c r="AR1" s="673"/>
-      <c r="AS1" s="673"/>
-      <c r="AT1" s="673"/>
-      <c r="AU1" s="673"/>
-      <c r="AV1" s="673"/>
-      <c r="AW1" s="693"/>
-      <c r="AX1" s="700" t="s">
+      <c r="AQ1" s="678"/>
+      <c r="AR1" s="678"/>
+      <c r="AS1" s="678"/>
+      <c r="AT1" s="678"/>
+      <c r="AU1" s="678"/>
+      <c r="AV1" s="678"/>
+      <c r="AW1" s="679"/>
+      <c r="AX1" s="686" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" s="701"/>
-      <c r="AZ1" s="701"/>
-      <c r="BA1" s="701"/>
-      <c r="BB1" s="701"/>
-      <c r="BC1" s="702"/>
-      <c r="BD1" s="703" t="s">
+      <c r="AY1" s="687"/>
+      <c r="AZ1" s="687"/>
+      <c r="BA1" s="687"/>
+      <c r="BB1" s="687"/>
+      <c r="BC1" s="688"/>
+      <c r="BD1" s="689" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="704"/>
-      <c r="BF1" s="704"/>
-      <c r="BG1" s="704"/>
-      <c r="BH1" s="704"/>
-      <c r="BI1" s="705"/>
-      <c r="BJ1" s="706" t="s">
+      <c r="BE1" s="690"/>
+      <c r="BF1" s="690"/>
+      <c r="BG1" s="690"/>
+      <c r="BH1" s="690"/>
+      <c r="BI1" s="691"/>
+      <c r="BJ1" s="692" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" s="707"/>
-      <c r="BL1" s="707"/>
-      <c r="BM1" s="707"/>
-      <c r="BN1" s="707"/>
-      <c r="BO1" s="707"/>
-      <c r="BP1" s="708"/>
-      <c r="BQ1" s="681" t="s">
+      <c r="BK1" s="693"/>
+      <c r="BL1" s="693"/>
+      <c r="BM1" s="693"/>
+      <c r="BN1" s="693"/>
+      <c r="BO1" s="693"/>
+      <c r="BP1" s="694"/>
+      <c r="BQ1" s="666" t="s">
         <v>57</v>
       </c>
-      <c r="BR1" s="682"/>
-      <c r="BS1" s="682"/>
-      <c r="BT1" s="682"/>
-      <c r="BU1" s="682"/>
-      <c r="BV1" s="682"/>
+      <c r="BR1" s="667"/>
+      <c r="BS1" s="667"/>
+      <c r="BT1" s="667"/>
+      <c r="BU1" s="667"/>
+      <c r="BV1" s="667"/>
       <c r="BW1" s="8"/>
       <c r="BX1" s="9"/>
-      <c r="BY1" s="683" t="s">
+      <c r="BY1" s="668" t="s">
         <v>58</v>
       </c>
-      <c r="BZ1" s="684"/>
-      <c r="CA1" s="684"/>
-      <c r="CB1" s="684"/>
-      <c r="CC1" s="684"/>
-      <c r="CD1" s="684"/>
-      <c r="CE1" s="684"/>
-      <c r="CF1" s="685"/>
-      <c r="CG1" s="685"/>
-      <c r="CH1" s="685"/>
-      <c r="CI1" s="685"/>
-      <c r="CJ1" s="685"/>
-      <c r="CK1" s="685"/>
-      <c r="CL1" s="685"/>
-      <c r="CM1" s="685"/>
-      <c r="CN1" s="685"/>
-      <c r="CO1" s="685"/>
-      <c r="CP1" s="685"/>
-      <c r="CQ1" s="685"/>
+      <c r="BZ1" s="669"/>
+      <c r="CA1" s="669"/>
+      <c r="CB1" s="669"/>
+      <c r="CC1" s="669"/>
+      <c r="CD1" s="669"/>
+      <c r="CE1" s="669"/>
+      <c r="CF1" s="670"/>
+      <c r="CG1" s="670"/>
+      <c r="CH1" s="670"/>
+      <c r="CI1" s="670"/>
+      <c r="CJ1" s="670"/>
+      <c r="CK1" s="670"/>
+      <c r="CL1" s="670"/>
+      <c r="CM1" s="670"/>
+      <c r="CN1" s="670"/>
+      <c r="CO1" s="670"/>
+      <c r="CP1" s="670"/>
+      <c r="CQ1" s="670"/>
     </row>
     <row r="2" spans="1:95" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -30976,18 +30985,18 @@
       <c r="G2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="686" t="s">
+      <c r="H2" s="671" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="687"/>
-      <c r="J2" s="687" t="s">
+      <c r="I2" s="672"/>
+      <c r="J2" s="672" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="687"/>
-      <c r="L2" s="687" t="s">
+      <c r="K2" s="672"/>
+      <c r="L2" s="672" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="688"/>
+      <c r="M2" s="673"/>
       <c r="N2" s="12" t="s">
         <v>59</v>
       </c>
@@ -31096,36 +31105,36 @@
       <c r="AW2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AX2" s="689" t="s">
+      <c r="AX2" s="674" t="s">
         <v>93</v>
       </c>
-      <c r="AY2" s="690"/>
-      <c r="AZ2" s="690"/>
-      <c r="BA2" s="690" t="s">
+      <c r="AY2" s="675"/>
+      <c r="AZ2" s="675"/>
+      <c r="BA2" s="675" t="s">
         <v>94</v>
       </c>
-      <c r="BB2" s="690"/>
-      <c r="BC2" s="691"/>
-      <c r="BD2" s="694" t="s">
+      <c r="BB2" s="675"/>
+      <c r="BC2" s="676"/>
+      <c r="BD2" s="680" t="s">
         <v>93</v>
       </c>
-      <c r="BE2" s="695"/>
-      <c r="BF2" s="695"/>
-      <c r="BG2" s="695" t="s">
+      <c r="BE2" s="681"/>
+      <c r="BF2" s="681"/>
+      <c r="BG2" s="681" t="s">
         <v>94</v>
       </c>
-      <c r="BH2" s="695"/>
-      <c r="BI2" s="696"/>
-      <c r="BJ2" s="697" t="s">
+      <c r="BH2" s="681"/>
+      <c r="BI2" s="682"/>
+      <c r="BJ2" s="683" t="s">
         <v>93</v>
       </c>
-      <c r="BK2" s="698"/>
-      <c r="BL2" s="698"/>
-      <c r="BM2" s="698" t="s">
+      <c r="BK2" s="684"/>
+      <c r="BL2" s="684"/>
+      <c r="BM2" s="684" t="s">
         <v>94</v>
       </c>
-      <c r="BN2" s="699"/>
-      <c r="BO2" s="699"/>
+      <c r="BN2" s="685"/>
+      <c r="BO2" s="685"/>
       <c r="BP2" s="24" t="s">
         <v>95</v>
       </c>
@@ -32032,6 +32041,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -32047,11 +32061,6 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:A14 A4:B4">
     <cfRule type="duplicateValues" dxfId="8" priority="1"/>
@@ -32090,124 +32099,124 @@
         <v>138</v>
       </c>
       <c r="L1" s="87"/>
-      <c r="M1" s="713" t="s">
+      <c r="M1" s="734" t="s">
         <v>139</v>
       </c>
-      <c r="N1" s="714" t="s">
+      <c r="N1" s="735" t="s">
         <v>140</v>
       </c>
-      <c r="O1" s="715"/>
-      <c r="P1" s="715"/>
-      <c r="Q1" s="715"/>
-      <c r="R1" s="716" t="s">
+      <c r="O1" s="736"/>
+      <c r="P1" s="736"/>
+      <c r="Q1" s="736"/>
+      <c r="R1" s="737" t="s">
         <v>141</v>
       </c>
-      <c r="S1" s="717"/>
-      <c r="T1" s="717"/>
-      <c r="U1" s="717"/>
-      <c r="V1" s="717"/>
-      <c r="W1" s="717"/>
-      <c r="X1" s="718"/>
-      <c r="Y1" s="719" t="s">
+      <c r="S1" s="729"/>
+      <c r="T1" s="729"/>
+      <c r="U1" s="729"/>
+      <c r="V1" s="729"/>
+      <c r="W1" s="729"/>
+      <c r="X1" s="738"/>
+      <c r="Y1" s="718" t="s">
         <v>142</v>
       </c>
-      <c r="Z1" s="704"/>
-      <c r="AA1" s="722" t="s">
+      <c r="Z1" s="690"/>
+      <c r="AA1" s="739" t="s">
         <v>143</v>
       </c>
-      <c r="AB1" s="724" t="s">
+      <c r="AB1" s="730" t="s">
         <v>144</v>
       </c>
-      <c r="AC1" s="732" t="s">
+      <c r="AC1" s="725" t="s">
         <v>145</v>
       </c>
-      <c r="AD1" s="733"/>
-      <c r="AE1" s="733"/>
-      <c r="AF1" s="734"/>
-      <c r="AG1" s="735" t="s">
+      <c r="AD1" s="726"/>
+      <c r="AE1" s="726"/>
+      <c r="AF1" s="727"/>
+      <c r="AG1" s="728" t="s">
         <v>146</v>
       </c>
-      <c r="AH1" s="717"/>
-      <c r="AI1" s="717"/>
-      <c r="AJ1" s="717"/>
-      <c r="AK1" s="717"/>
-      <c r="AL1" s="717"/>
-      <c r="AM1" s="717"/>
-      <c r="AN1" s="717"/>
-      <c r="AO1" s="724" t="s">
+      <c r="AH1" s="729"/>
+      <c r="AI1" s="729"/>
+      <c r="AJ1" s="729"/>
+      <c r="AK1" s="729"/>
+      <c r="AL1" s="729"/>
+      <c r="AM1" s="729"/>
+      <c r="AN1" s="729"/>
+      <c r="AO1" s="730" t="s">
         <v>147</v>
       </c>
-      <c r="AP1" s="719" t="s">
+      <c r="AP1" s="718" t="s">
         <v>148</v>
       </c>
-      <c r="AQ1" s="704"/>
-      <c r="AR1" s="704"/>
-      <c r="AS1" s="705"/>
-      <c r="AT1" s="736" t="s">
+      <c r="AQ1" s="690"/>
+      <c r="AR1" s="690"/>
+      <c r="AS1" s="691"/>
+      <c r="AT1" s="732" t="s">
         <v>149</v>
       </c>
-      <c r="AU1" s="737"/>
-      <c r="AV1" s="737"/>
-      <c r="AW1" s="737"/>
-      <c r="AX1" s="737"/>
-      <c r="AY1" s="737"/>
-      <c r="AZ1" s="737"/>
-      <c r="BA1" s="737"/>
-      <c r="BB1" s="737"/>
-      <c r="BC1" s="737"/>
-      <c r="BD1" s="737"/>
-      <c r="BE1" s="737"/>
-      <c r="BF1" s="737"/>
-      <c r="BG1" s="737"/>
-      <c r="BH1" s="737"/>
-      <c r="BI1" s="737"/>
-      <c r="BJ1" s="737"/>
-      <c r="BK1" s="737"/>
-      <c r="BL1" s="737"/>
-      <c r="BM1" s="737"/>
-      <c r="BN1" s="737"/>
-      <c r="BO1" s="737"/>
-      <c r="BP1" s="737"/>
-      <c r="BQ1" s="737"/>
-      <c r="BR1" s="737"/>
-      <c r="BS1" s="737"/>
-      <c r="BT1" s="737"/>
-      <c r="BU1" s="737"/>
-      <c r="BV1" s="737"/>
-      <c r="BW1" s="724" t="s">
+      <c r="AU1" s="733"/>
+      <c r="AV1" s="733"/>
+      <c r="AW1" s="733"/>
+      <c r="AX1" s="733"/>
+      <c r="AY1" s="733"/>
+      <c r="AZ1" s="733"/>
+      <c r="BA1" s="733"/>
+      <c r="BB1" s="733"/>
+      <c r="BC1" s="733"/>
+      <c r="BD1" s="733"/>
+      <c r="BE1" s="733"/>
+      <c r="BF1" s="733"/>
+      <c r="BG1" s="733"/>
+      <c r="BH1" s="733"/>
+      <c r="BI1" s="733"/>
+      <c r="BJ1" s="733"/>
+      <c r="BK1" s="733"/>
+      <c r="BL1" s="733"/>
+      <c r="BM1" s="733"/>
+      <c r="BN1" s="733"/>
+      <c r="BO1" s="733"/>
+      <c r="BP1" s="733"/>
+      <c r="BQ1" s="733"/>
+      <c r="BR1" s="733"/>
+      <c r="BS1" s="733"/>
+      <c r="BT1" s="733"/>
+      <c r="BU1" s="733"/>
+      <c r="BV1" s="733"/>
+      <c r="BW1" s="730" t="s">
         <v>150</v>
       </c>
-      <c r="BX1" s="719" t="s">
+      <c r="BX1" s="718" t="s">
         <v>151</v>
       </c>
-      <c r="BY1" s="704"/>
-      <c r="BZ1" s="704"/>
-      <c r="CA1" s="705"/>
-      <c r="CB1" s="726" t="s">
+      <c r="BY1" s="690"/>
+      <c r="BZ1" s="690"/>
+      <c r="CA1" s="691"/>
+      <c r="CB1" s="719" t="s">
         <v>52</v>
       </c>
-      <c r="CC1" s="726"/>
-      <c r="CD1" s="726"/>
-      <c r="CE1" s="726"/>
-      <c r="CF1" s="726"/>
-      <c r="CG1" s="726"/>
-      <c r="CH1" s="726"/>
-      <c r="CI1" s="726"/>
-      <c r="CJ1" s="726"/>
-      <c r="CK1" s="726"/>
-      <c r="CL1" s="726"/>
-      <c r="CM1" s="726"/>
+      <c r="CC1" s="719"/>
+      <c r="CD1" s="719"/>
+      <c r="CE1" s="719"/>
+      <c r="CF1" s="719"/>
+      <c r="CG1" s="719"/>
+      <c r="CH1" s="719"/>
+      <c r="CI1" s="719"/>
+      <c r="CJ1" s="719"/>
+      <c r="CK1" s="719"/>
+      <c r="CL1" s="719"/>
+      <c r="CM1" s="719"/>
       <c r="CN1" s="88"/>
-      <c r="CO1" s="727" t="s">
+      <c r="CO1" s="720" t="s">
         <v>57</v>
       </c>
-      <c r="CP1" s="673"/>
-      <c r="CQ1" s="673"/>
-      <c r="CR1" s="673"/>
-      <c r="CS1" s="673"/>
-      <c r="CT1" s="673"/>
-      <c r="CU1" s="673"/>
-      <c r="CV1" s="693"/>
+      <c r="CP1" s="678"/>
+      <c r="CQ1" s="678"/>
+      <c r="CR1" s="678"/>
+      <c r="CS1" s="678"/>
+      <c r="CT1" s="678"/>
+      <c r="CU1" s="678"/>
+      <c r="CV1" s="679"/>
     </row>
     <row r="2" spans="1:100" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" s="89" t="s">
@@ -32246,7 +32255,7 @@
       <c r="L2" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="713"/>
+      <c r="M2" s="734"/>
       <c r="N2" s="94" t="s">
         <v>156</v>
       </c>
@@ -32262,22 +32271,22 @@
       <c r="R2" s="95" t="s">
         <v>436</v>
       </c>
-      <c r="S2" s="728" t="s">
+      <c r="S2" s="721" t="s">
         <v>159</v>
       </c>
-      <c r="T2" s="699"/>
-      <c r="U2" s="729" t="s">
+      <c r="T2" s="685"/>
+      <c r="U2" s="722" t="s">
         <v>67</v>
       </c>
-      <c r="V2" s="729"/>
-      <c r="W2" s="729" t="s">
+      <c r="V2" s="722"/>
+      <c r="W2" s="722" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="730"/>
-      <c r="Y2" s="720"/>
-      <c r="Z2" s="721"/>
-      <c r="AA2" s="723"/>
-      <c r="AB2" s="725"/>
+      <c r="X2" s="723"/>
+      <c r="Y2" s="712"/>
+      <c r="Z2" s="713"/>
+      <c r="AA2" s="740"/>
+      <c r="AB2" s="731"/>
       <c r="AC2" s="96" t="s">
         <v>160</v>
       </c>
@@ -32290,81 +32299,81 @@
       <c r="AF2" s="96" t="s">
         <v>163</v>
       </c>
-      <c r="AG2" s="731" t="s">
+      <c r="AG2" s="724" t="s">
         <v>164</v>
       </c>
-      <c r="AH2" s="711"/>
-      <c r="AI2" s="711" t="s">
+      <c r="AH2" s="710"/>
+      <c r="AI2" s="710" t="s">
         <v>165</v>
       </c>
-      <c r="AJ2" s="711"/>
-      <c r="AK2" s="711" t="s">
+      <c r="AJ2" s="710"/>
+      <c r="AK2" s="710" t="s">
         <v>166</v>
       </c>
-      <c r="AL2" s="711"/>
+      <c r="AL2" s="710"/>
       <c r="AM2" s="97" t="s">
         <v>167</v>
       </c>
       <c r="AN2" s="97" t="s">
         <v>168</v>
       </c>
-      <c r="AO2" s="725"/>
-      <c r="AP2" s="720" t="s">
+      <c r="AO2" s="731"/>
+      <c r="AP2" s="712" t="s">
         <v>169</v>
       </c>
-      <c r="AQ2" s="721"/>
-      <c r="AR2" s="709" t="s">
+      <c r="AQ2" s="713"/>
+      <c r="AR2" s="714" t="s">
         <v>170</v>
       </c>
-      <c r="AS2" s="710"/>
-      <c r="AT2" s="711" t="s">
+      <c r="AS2" s="715"/>
+      <c r="AT2" s="710" t="s">
         <v>171</v>
       </c>
-      <c r="AU2" s="711"/>
-      <c r="AV2" s="712" t="s">
+      <c r="AU2" s="710"/>
+      <c r="AV2" s="711" t="s">
         <v>172</v>
       </c>
-      <c r="AW2" s="712"/>
-      <c r="AX2" s="712" t="s">
+      <c r="AW2" s="711"/>
+      <c r="AX2" s="711" t="s">
         <v>173</v>
       </c>
-      <c r="AY2" s="712"/>
+      <c r="AY2" s="711"/>
       <c r="AZ2" s="97" t="s">
         <v>174</v>
       </c>
       <c r="BA2" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="BB2" s="711" t="s">
+      <c r="BB2" s="710" t="s">
         <v>176</v>
       </c>
-      <c r="BC2" s="711"/>
-      <c r="BD2" s="712" t="s">
+      <c r="BC2" s="710"/>
+      <c r="BD2" s="711" t="s">
         <v>177</v>
       </c>
-      <c r="BE2" s="712"/>
-      <c r="BF2" s="712" t="s">
+      <c r="BE2" s="711"/>
+      <c r="BF2" s="711" t="s">
         <v>178</v>
       </c>
-      <c r="BG2" s="712"/>
+      <c r="BG2" s="711"/>
       <c r="BH2" s="97" t="s">
         <v>179</v>
       </c>
       <c r="BI2" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="BJ2" s="711" t="s">
+      <c r="BJ2" s="710" t="s">
         <v>181</v>
       </c>
-      <c r="BK2" s="711"/>
-      <c r="BL2" s="712" t="s">
+      <c r="BK2" s="710"/>
+      <c r="BL2" s="711" t="s">
         <v>182</v>
       </c>
-      <c r="BM2" s="712"/>
-      <c r="BN2" s="712" t="s">
+      <c r="BM2" s="711"/>
+      <c r="BN2" s="711" t="s">
         <v>183</v>
       </c>
-      <c r="BO2" s="712"/>
+      <c r="BO2" s="711"/>
       <c r="BP2" s="97" t="s">
         <v>184</v>
       </c>
@@ -32386,15 +32395,15 @@
       <c r="BV2" s="97" t="s">
         <v>190</v>
       </c>
-      <c r="BW2" s="725"/>
-      <c r="BX2" s="720" t="s">
+      <c r="BW2" s="731"/>
+      <c r="BX2" s="712" t="s">
         <v>169</v>
       </c>
-      <c r="BY2" s="721"/>
-      <c r="BZ2" s="709" t="s">
+      <c r="BY2" s="713"/>
+      <c r="BZ2" s="714" t="s">
         <v>170</v>
       </c>
-      <c r="CA2" s="710"/>
+      <c r="CA2" s="715"/>
       <c r="CB2" s="20" t="s">
         <v>74</v>
       </c>
@@ -32434,22 +32443,22 @@
       <c r="CN2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="CO2" s="740" t="s">
+      <c r="CO2" s="716" t="s">
         <v>191</v>
       </c>
-      <c r="CP2" s="741"/>
-      <c r="CQ2" s="738" t="s">
+      <c r="CP2" s="717"/>
+      <c r="CQ2" s="708" t="s">
         <v>192</v>
       </c>
-      <c r="CR2" s="738"/>
-      <c r="CS2" s="741" t="s">
+      <c r="CR2" s="708"/>
+      <c r="CS2" s="717" t="s">
         <v>193</v>
       </c>
-      <c r="CT2" s="741"/>
-      <c r="CU2" s="738" t="s">
+      <c r="CT2" s="717"/>
+      <c r="CU2" s="708" t="s">
         <v>194</v>
       </c>
-      <c r="CV2" s="739"/>
+      <c r="CV2" s="709"/>
     </row>
     <row r="3" spans="1:100" ht="27" x14ac:dyDescent="0.25">
       <c r="A3" s="99" t="s">
@@ -37755,18 +37764,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="BX1:CA1"/>
     <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CO1:CV1"/>
@@ -37783,16 +37790,18 @@
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
     <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="CS2:CT2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37802,7 +37811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
@@ -37845,8 +37854,8 @@
       <c r="B2" s="209" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="742"/>
-      <c r="D2" s="742"/>
+      <c r="C2" s="748"/>
+      <c r="D2" s="748"/>
       <c r="E2" s="207"/>
       <c r="F2" s="207"/>
       <c r="G2" s="207"/>
@@ -37971,32 +37980,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="206"/>
-      <c r="B7" s="743" t="s">
+      <c r="B7" s="749" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="743"/>
-      <c r="D7" s="743"/>
+      <c r="C7" s="749"/>
+      <c r="D7" s="749"/>
       <c r="E7" s="207"/>
       <c r="F7" s="207"/>
       <c r="G7" s="207"/>
       <c r="H7" s="207"/>
       <c r="I7" s="207"/>
-      <c r="J7" s="743" t="s">
+      <c r="J7" s="749" t="s">
         <v>218</v>
       </c>
-      <c r="K7" s="743"/>
-      <c r="L7" s="743"/>
+      <c r="K7" s="749"/>
+      <c r="L7" s="749"/>
       <c r="M7" s="207"/>
       <c r="N7" s="207"/>
       <c r="O7" s="207"/>
       <c r="P7" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="Q7" s="743" t="s">
+      <c r="Q7" s="749" t="s">
         <v>218</v>
       </c>
-      <c r="R7" s="743"/>
-      <c r="S7" s="743"/>
+      <c r="R7" s="749"/>
+      <c r="S7" s="749"/>
       <c r="T7" s="207"/>
       <c r="U7" s="221" t="s">
         <v>220</v>
@@ -38126,10 +38135,10 @@
       </c>
       <c r="C11" s="227"/>
       <c r="D11" s="227"/>
-      <c r="E11" s="746" t="s">
+      <c r="E11" s="741" t="s">
         <v>228</v>
       </c>
-      <c r="F11" s="747"/>
+      <c r="F11" s="742"/>
       <c r="G11" s="228"/>
       <c r="H11" s="228"/>
       <c r="I11" s="228"/>
@@ -38138,10 +38147,10 @@
       </c>
       <c r="K11" s="207"/>
       <c r="L11" s="207"/>
-      <c r="M11" s="749" t="s">
+      <c r="M11" s="746" t="s">
         <v>228</v>
       </c>
-      <c r="N11" s="750"/>
+      <c r="N11" s="747"/>
       <c r="O11" s="228"/>
       <c r="P11" s="228"/>
       <c r="Q11" s="226" t="s">
@@ -38149,10 +38158,10 @@
       </c>
       <c r="R11" s="227"/>
       <c r="S11" s="227"/>
-      <c r="T11" s="746" t="s">
+      <c r="T11" s="741" t="s">
         <v>228</v>
       </c>
-      <c r="U11" s="747"/>
+      <c r="U11" s="742"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="206"/>
@@ -38387,10 +38396,10 @@
       </c>
       <c r="C20" s="569"/>
       <c r="D20" s="255"/>
-      <c r="E20" s="746" t="s">
+      <c r="E20" s="741" t="s">
         <v>235</v>
       </c>
-      <c r="F20" s="747"/>
+      <c r="F20" s="742"/>
       <c r="G20" s="236"/>
       <c r="H20" s="236"/>
       <c r="I20" s="207"/>
@@ -38399,10 +38408,10 @@
       </c>
       <c r="K20" s="569"/>
       <c r="L20" s="255"/>
-      <c r="M20" s="746" t="s">
+      <c r="M20" s="741" t="s">
         <v>235</v>
       </c>
-      <c r="N20" s="747"/>
+      <c r="N20" s="742"/>
       <c r="O20" s="246"/>
       <c r="P20" s="246"/>
       <c r="Q20" s="226" t="s">
@@ -38410,10 +38419,10 @@
       </c>
       <c r="R20" s="569"/>
       <c r="S20" s="255"/>
-      <c r="T20" s="746" t="s">
+      <c r="T20" s="741" t="s">
         <v>235</v>
       </c>
-      <c r="U20" s="747"/>
+      <c r="U20" s="742"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="206"/>
@@ -38677,10 +38686,10 @@
       </c>
       <c r="C30" s="569"/>
       <c r="D30" s="255"/>
-      <c r="E30" s="746" t="s">
+      <c r="E30" s="741" t="s">
         <v>235</v>
       </c>
-      <c r="F30" s="747"/>
+      <c r="F30" s="742"/>
       <c r="G30" s="236"/>
       <c r="H30" s="236"/>
       <c r="I30" s="207"/>
@@ -38689,10 +38698,10 @@
       </c>
       <c r="K30" s="569"/>
       <c r="L30" s="255"/>
-      <c r="M30" s="746" t="s">
+      <c r="M30" s="741" t="s">
         <v>235</v>
       </c>
-      <c r="N30" s="747"/>
+      <c r="N30" s="742"/>
       <c r="O30" s="246"/>
       <c r="P30" s="246"/>
       <c r="Q30" s="226" t="s">
@@ -38700,10 +38709,10 @@
       </c>
       <c r="R30" s="569"/>
       <c r="S30" s="255"/>
-      <c r="T30" s="746" t="s">
+      <c r="T30" s="741" t="s">
         <v>235</v>
       </c>
-      <c r="U30" s="747"/>
+      <c r="U30" s="742"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="269"/>
@@ -39026,11 +39035,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="206"/>
-      <c r="B42" s="748"/>
-      <c r="C42" s="748"/>
-      <c r="D42" s="748"/>
-      <c r="E42" s="748"/>
-      <c r="F42" s="748"/>
+      <c r="B42" s="743"/>
+      <c r="C42" s="743"/>
+      <c r="D42" s="743"/>
+      <c r="E42" s="743"/>
+      <c r="F42" s="743"/>
       <c r="G42" s="246"/>
       <c r="H42" s="207"/>
       <c r="I42" s="246"/>
@@ -39174,6 +39183,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -39185,15 +39203,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39204,8 +39213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39226,8 +39235,8 @@
       <c r="B3" s="292" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="751"/>
-      <c r="D3" s="751"/>
+      <c r="C3" s="750"/>
+      <c r="D3" s="750"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="293"/>
@@ -39260,10 +39269,10 @@
       <c r="D10" s="301" t="s">
         <v>255</v>
       </c>
-      <c r="E10" s="752" t="s">
+      <c r="E10" s="751" t="s">
         <v>256</v>
       </c>
-      <c r="F10" s="753"/>
+      <c r="F10" s="752"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="302" t="s">
@@ -39299,8 +39308,8 @@
       </c>
       <c r="C13" s="571"/>
       <c r="D13" s="579"/>
-      <c r="E13" s="579"/>
-      <c r="F13" s="576"/>
+      <c r="E13" s="804"/>
+      <c r="F13" s="805"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="586" t="s">
@@ -39308,8 +39317,8 @@
       </c>
       <c r="C14" s="587"/>
       <c r="D14" s="588"/>
-      <c r="E14" s="589"/>
-      <c r="F14" s="577"/>
+      <c r="E14" s="806"/>
+      <c r="F14" s="807"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="309"/>
@@ -39340,7 +39349,7 @@
       <c r="B18" s="586" t="s">
         <v>262</v>
       </c>
-      <c r="C18" s="590"/>
+      <c r="C18" s="589"/>
       <c r="D18" s="588"/>
       <c r="E18" s="588"/>
       <c r="F18" s="577"/>
@@ -39380,10 +39389,10 @@
       <c r="F22" s="576"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="598"/>
-      <c r="C23" s="597"/>
-      <c r="D23" s="596"/>
-      <c r="E23" s="595"/>
+      <c r="B23" s="597"/>
+      <c r="C23" s="596"/>
+      <c r="D23" s="595"/>
+      <c r="E23" s="594"/>
       <c r="F23" s="577"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -39414,10 +39423,10 @@
       <c r="D30" s="313" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="752" t="s">
+      <c r="E30" s="751" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="753"/>
+      <c r="F30" s="752"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="302" t="s">
@@ -39453,8 +39462,8 @@
       </c>
       <c r="C33" s="571"/>
       <c r="D33" s="579"/>
-      <c r="E33" s="579"/>
-      <c r="F33" s="576"/>
+      <c r="E33" s="804"/>
+      <c r="F33" s="805"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="586" t="s">
@@ -39462,8 +39471,8 @@
       </c>
       <c r="C34" s="587"/>
       <c r="D34" s="588"/>
-      <c r="E34" s="589"/>
-      <c r="F34" s="577"/>
+      <c r="E34" s="806"/>
+      <c r="F34" s="807"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="309"/>
@@ -39491,10 +39500,10 @@
       <c r="F37" s="576"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="591" t="s">
+      <c r="B38" s="590" t="s">
         <v>262</v>
       </c>
-      <c r="C38" s="592"/>
+      <c r="C38" s="591"/>
       <c r="D38" s="588"/>
       <c r="E38" s="588"/>
       <c r="F38" s="577"/>
@@ -39535,9 +39544,9 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="315"/>
-      <c r="C43" s="594"/>
+      <c r="C43" s="593"/>
       <c r="D43" s="585"/>
-      <c r="E43" s="593"/>
+      <c r="E43" s="592"/>
       <c r="F43" s="577"/>
     </row>
     <row r="46" spans="2:6" ht="21" x14ac:dyDescent="0.35">
@@ -39565,10 +39574,10 @@
       <c r="D49" s="313" t="s">
         <v>255</v>
       </c>
-      <c r="E49" s="752" t="s">
+      <c r="E49" s="751" t="s">
         <v>256</v>
       </c>
-      <c r="F49" s="753"/>
+      <c r="F49" s="752"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="302" t="s">
@@ -39604,8 +39613,8 @@
       </c>
       <c r="C52" s="571"/>
       <c r="D52" s="579"/>
-      <c r="E52" s="579"/>
-      <c r="F52" s="576"/>
+      <c r="E52" s="804"/>
+      <c r="F52" s="805"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="586" t="s">
@@ -39613,8 +39622,8 @@
       </c>
       <c r="C53" s="587"/>
       <c r="D53" s="588"/>
-      <c r="E53" s="589"/>
-      <c r="F53" s="577"/>
+      <c r="E53" s="806"/>
+      <c r="F53" s="807"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="309"/>
@@ -39645,7 +39654,7 @@
       <c r="B57" s="586" t="s">
         <v>262</v>
       </c>
-      <c r="C57" s="590"/>
+      <c r="C57" s="589"/>
       <c r="D57" s="588"/>
       <c r="E57" s="588"/>
       <c r="F57" s="577"/>
@@ -39686,9 +39695,9 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="315"/>
-      <c r="C62" s="594"/>
-      <c r="D62" s="599"/>
-      <c r="E62" s="595"/>
+      <c r="C62" s="593"/>
+      <c r="D62" s="598"/>
+      <c r="E62" s="594"/>
       <c r="F62" s="577"/>
     </row>
   </sheetData>
@@ -39706,8 +39715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39736,8 +39745,8 @@
       </c>
       <c r="C2" s="209"/>
       <c r="D2" s="209"/>
-      <c r="E2" s="742"/>
-      <c r="F2" s="742"/>
+      <c r="E2" s="748"/>
+      <c r="F2" s="748"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="208"/>
@@ -39769,13 +39778,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="206"/>
-      <c r="B6" s="743" t="s">
+      <c r="B6" s="749" t="s">
         <v>268</v>
       </c>
-      <c r="C6" s="743"/>
-      <c r="D6" s="743"/>
-      <c r="E6" s="743"/>
-      <c r="F6" s="743"/>
+      <c r="C6" s="749"/>
+      <c r="D6" s="749"/>
+      <c r="E6" s="749"/>
+      <c r="F6" s="749"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="206"/>
@@ -39787,27 +39796,27 @@
     </row>
     <row r="8" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="206"/>
-      <c r="B8" s="606" t="s">
+      <c r="B8" s="605" t="s">
         <v>221</v>
       </c>
-      <c r="C8" s="754" t="s">
+      <c r="C8" s="753" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="755"/>
-      <c r="E8" s="756" t="s">
+      <c r="D8" s="754"/>
+      <c r="E8" s="755" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="755"/>
+      <c r="F8" s="754"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="206"/>
-      <c r="B9" s="607" t="s">
+      <c r="B9" s="606" t="s">
         <v>214</v>
       </c>
-      <c r="C9" s="604" t="s">
+      <c r="C9" s="603" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="605" t="s">
+      <c r="D9" s="604" t="s">
         <v>226</v>
       </c>
       <c r="E9" s="317" t="s">
@@ -39819,55 +39828,55 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="319"/>
-      <c r="B10" s="612" t="s">
+      <c r="B10" s="611" t="s">
         <v>269</v>
       </c>
       <c r="C10" s="320"/>
-      <c r="D10" s="620"/>
+      <c r="D10" s="619"/>
       <c r="E10" s="320"/>
-      <c r="F10" s="626"/>
+      <c r="F10" s="625"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="319"/>
-      <c r="B11" s="613" t="s">
+      <c r="B11" s="612" t="s">
         <v>270</v>
       </c>
       <c r="C11" s="324"/>
-      <c r="D11" s="621"/>
-      <c r="E11" s="601"/>
-      <c r="F11" s="627"/>
+      <c r="D11" s="620"/>
+      <c r="E11" s="600"/>
+      <c r="F11" s="626"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="322"/>
-      <c r="B12" s="608" t="s">
+      <c r="B12" s="607" t="s">
         <v>258</v>
       </c>
-      <c r="C12" s="603"/>
-      <c r="D12" s="602"/>
-      <c r="E12" s="603"/>
-      <c r="F12" s="602"/>
+      <c r="C12" s="602"/>
+      <c r="D12" s="601"/>
+      <c r="E12" s="602"/>
+      <c r="F12" s="601"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="322"/>
       <c r="B13" s="238"/>
-      <c r="C13" s="614"/>
-      <c r="D13" s="622"/>
+      <c r="C13" s="613"/>
+      <c r="D13" s="621"/>
       <c r="E13" s="327"/>
-      <c r="F13" s="600"/>
+      <c r="F13" s="599"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="319"/>
       <c r="B14" s="326" t="s">
         <v>271</v>
       </c>
-      <c r="C14" s="615"/>
-      <c r="D14" s="623"/>
-      <c r="E14" s="618"/>
-      <c r="F14" s="628"/>
+      <c r="C14" s="614"/>
+      <c r="D14" s="622"/>
+      <c r="E14" s="617"/>
+      <c r="F14" s="627"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="322"/>
-      <c r="B15" s="609" t="s">
+      <c r="B15" s="608" t="s">
         <v>264</v>
       </c>
       <c r="C15" s="321"/>
@@ -39877,35 +39886,35 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="322"/>
-      <c r="B16" s="608" t="s">
+      <c r="B16" s="607" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="603"/>
-      <c r="D16" s="602"/>
-      <c r="E16" s="603"/>
-      <c r="F16" s="602"/>
+      <c r="C16" s="602"/>
+      <c r="D16" s="601"/>
+      <c r="E16" s="602"/>
+      <c r="F16" s="601"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="322"/>
       <c r="B17" s="329"/>
-      <c r="C17" s="616"/>
-      <c r="D17" s="624"/>
-      <c r="E17" s="616"/>
-      <c r="F17" s="629"/>
+      <c r="C17" s="615"/>
+      <c r="D17" s="623"/>
+      <c r="E17" s="615"/>
+      <c r="F17" s="628"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="319"/>
       <c r="B18" s="326" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="615"/>
-      <c r="D18" s="623"/>
-      <c r="E18" s="618"/>
-      <c r="F18" s="628"/>
+      <c r="C18" s="614"/>
+      <c r="D18" s="622"/>
+      <c r="E18" s="617"/>
+      <c r="F18" s="627"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="322"/>
-      <c r="B19" s="609" t="s">
+      <c r="B19" s="608" t="s">
         <v>264</v>
       </c>
       <c r="C19" s="321"/>
@@ -39915,7 +39924,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="322"/>
-      <c r="B20" s="610" t="s">
+      <c r="B20" s="609" t="s">
         <v>262</v>
       </c>
       <c r="C20" s="327"/>
@@ -39925,19 +39934,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="322"/>
-      <c r="B21" s="611"/>
-      <c r="C21" s="617"/>
-      <c r="D21" s="625"/>
-      <c r="E21" s="619"/>
-      <c r="F21" s="630"/>
+      <c r="B21" s="610"/>
+      <c r="C21" s="616"/>
+      <c r="D21" s="624"/>
+      <c r="E21" s="618"/>
+      <c r="F21" s="629"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="206"/>
-      <c r="B22" s="748"/>
-      <c r="C22" s="748"/>
-      <c r="D22" s="748"/>
-      <c r="E22" s="748"/>
-      <c r="F22" s="748"/>
+      <c r="B22" s="743"/>
+      <c r="C22" s="743"/>
+      <c r="D22" s="743"/>
+      <c r="E22" s="743"/>
+      <c r="F22" s="743"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="206"/>
@@ -40000,13 +40009,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="B2" s="757" t="s">
+      <c r="B2" s="756" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="758" t="s">
+      <c r="C2" s="757" t="s">
         <v>276</v>
       </c>
-      <c r="D2" s="758" t="s">
+      <c r="D2" s="757" t="s">
         <v>154</v>
       </c>
       <c r="E2" s="330" t="s">
@@ -40041,9 +40050,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="757"/>
-      <c r="C3" s="759"/>
-      <c r="D3" s="759"/>
+      <c r="B3" s="756"/>
+      <c r="C3" s="758"/>
+      <c r="D3" s="758"/>
       <c r="E3" s="332" t="s">
         <v>285</v>
       </c>
@@ -40076,7 +40085,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="760" t="s">
+      <c r="B4" s="759" t="s">
         <v>288</v>
       </c>
       <c r="C4" s="334" t="s">
@@ -40095,7 +40104,7 @@
       <c r="N4" s="336"/>
     </row>
     <row r="5" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="760"/>
+      <c r="B5" s="759"/>
       <c r="C5" s="334" t="s">
         <v>62</v>
       </c>
@@ -40112,7 +40121,7 @@
       <c r="N5" s="336"/>
     </row>
     <row r="6" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="761"/>
+      <c r="B6" s="760"/>
       <c r="C6" s="337" t="s">
         <v>278</v>
       </c>
@@ -40173,16 +40182,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="762" t="s">
+      <c r="A1" s="761" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="763"/>
-      <c r="C1" s="764"/>
-      <c r="D1" s="765" t="s">
+      <c r="B1" s="762"/>
+      <c r="C1" s="763"/>
+      <c r="D1" s="764" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="765"/>
-      <c r="F1" s="766"/>
+      <c r="E1" s="764"/>
+      <c r="F1" s="765"/>
       <c r="G1" s="347" t="s">
         <v>291</v>
       </c>
@@ -40190,7 +40199,7 @@
       <c r="I1" s="417"/>
       <c r="J1" s="417"/>
       <c r="K1" s="348"/>
-      <c r="L1" s="767" t="s">
+      <c r="L1" s="766" t="s">
         <v>292</v>
       </c>
     </row>
@@ -40228,7 +40237,7 @@
       <c r="K2" s="357" t="s">
         <v>296</v>
       </c>
-      <c r="L2" s="768"/>
+      <c r="L2" s="767"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="358"/>
@@ -40236,46 +40245,46 @@
       <c r="C3" s="360" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="769" t="s">
+      <c r="D3" s="768" t="s">
         <v>297</v>
       </c>
-      <c r="E3" s="770"/>
-      <c r="F3" s="771"/>
-      <c r="G3" s="772" t="s">
+      <c r="E3" s="769"/>
+      <c r="F3" s="770"/>
+      <c r="G3" s="771" t="s">
         <v>297</v>
       </c>
-      <c r="H3" s="773"/>
-      <c r="I3" s="773"/>
-      <c r="J3" s="773"/>
-      <c r="K3" s="774"/>
-      <c r="L3" s="768"/>
+      <c r="H3" s="772"/>
+      <c r="I3" s="772"/>
+      <c r="J3" s="772"/>
+      <c r="K3" s="773"/>
+      <c r="L3" s="767"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="418"/>
       <c r="B4" s="419"/>
       <c r="C4" s="420"/>
-      <c r="D4" s="631"/>
-      <c r="E4" s="633"/>
-      <c r="F4" s="633"/>
-      <c r="G4" s="633"/>
-      <c r="H4" s="633"/>
-      <c r="I4" s="633"/>
-      <c r="J4" s="633"/>
-      <c r="K4" s="633"/>
+      <c r="D4" s="630"/>
+      <c r="E4" s="632"/>
+      <c r="F4" s="632"/>
+      <c r="G4" s="632"/>
+      <c r="H4" s="632"/>
+      <c r="I4" s="632"/>
+      <c r="J4" s="632"/>
+      <c r="K4" s="632"/>
       <c r="L4" s="421"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="422"/>
       <c r="B5" s="423"/>
       <c r="C5" s="424"/>
-      <c r="D5" s="632"/>
-      <c r="E5" s="634"/>
-      <c r="F5" s="632"/>
-      <c r="G5" s="634"/>
-      <c r="H5" s="634"/>
-      <c r="I5" s="634"/>
-      <c r="J5" s="634"/>
-      <c r="K5" s="634"/>
+      <c r="D5" s="631"/>
+      <c r="E5" s="633"/>
+      <c r="F5" s="631"/>
+      <c r="G5" s="633"/>
+      <c r="H5" s="633"/>
+      <c r="I5" s="633"/>
+      <c r="J5" s="633"/>
+      <c r="K5" s="633"/>
       <c r="L5" s="425"/>
     </row>
   </sheetData>
@@ -40301,23 +40310,23 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="667" t="s">
+      <c r="A1" s="695" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="668"/>
-      <c r="C1" s="668"/>
-      <c r="D1" s="668"/>
+      <c r="B1" s="696"/>
+      <c r="C1" s="696"/>
+      <c r="D1" s="696"/>
       <c r="E1" s="361"/>
-      <c r="F1" s="780" t="s">
+      <c r="F1" s="779" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="781"/>
-      <c r="H1" s="781"/>
+      <c r="G1" s="780"/>
+      <c r="H1" s="780"/>
       <c r="I1" s="362"/>
       <c r="J1" s="363"/>
       <c r="K1" s="362"/>
       <c r="L1" s="364"/>
-      <c r="M1" s="775" t="s">
+      <c r="M1" s="774" t="s">
         <v>299</v>
       </c>
       <c r="N1" s="365"/>
@@ -40329,19 +40338,19 @@
       <c r="R1" s="363"/>
       <c r="S1" s="362"/>
       <c r="T1" s="364"/>
-      <c r="U1" s="775" t="s">
+      <c r="U1" s="774" t="s">
         <v>301</v>
       </c>
       <c r="V1" s="365"/>
-      <c r="W1" s="782" t="s">
+      <c r="W1" s="781" t="s">
         <v>302</v>
       </c>
-      <c r="X1" s="782"/>
-      <c r="Y1" s="782"/>
-      <c r="Z1" s="782"/>
-      <c r="AA1" s="782"/>
-      <c r="AB1" s="783"/>
-      <c r="AC1" s="775" t="s">
+      <c r="X1" s="781"/>
+      <c r="Y1" s="781"/>
+      <c r="Z1" s="781"/>
+      <c r="AA1" s="781"/>
+      <c r="AB1" s="782"/>
+      <c r="AC1" s="774" t="s">
         <v>303</v>
       </c>
     </row>
@@ -40355,52 +40364,52 @@
       <c r="C2" s="367" t="s">
         <v>305</v>
       </c>
-      <c r="D2" s="777" t="s">
+      <c r="D2" s="776" t="s">
         <v>306</v>
       </c>
-      <c r="E2" s="777"/>
+      <c r="E2" s="776"/>
       <c r="F2" s="368"/>
-      <c r="G2" s="778" t="s">
+      <c r="G2" s="777" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="778"/>
-      <c r="I2" s="778" t="s">
+      <c r="H2" s="777"/>
+      <c r="I2" s="777" t="s">
         <v>165</v>
       </c>
-      <c r="J2" s="778"/>
-      <c r="K2" s="778" t="s">
+      <c r="J2" s="777"/>
+      <c r="K2" s="777" t="s">
         <v>166</v>
       </c>
-      <c r="L2" s="779"/>
-      <c r="M2" s="776"/>
+      <c r="L2" s="778"/>
+      <c r="M2" s="775"/>
       <c r="N2" s="369"/>
-      <c r="O2" s="778" t="s">
+      <c r="O2" s="777" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="778"/>
-      <c r="Q2" s="778" t="s">
+      <c r="P2" s="777"/>
+      <c r="Q2" s="777" t="s">
         <v>165</v>
       </c>
-      <c r="R2" s="778"/>
-      <c r="S2" s="778" t="s">
+      <c r="R2" s="777"/>
+      <c r="S2" s="777" t="s">
         <v>166</v>
       </c>
-      <c r="T2" s="779"/>
-      <c r="U2" s="776"/>
+      <c r="T2" s="778"/>
+      <c r="U2" s="775"/>
       <c r="V2" s="369"/>
-      <c r="W2" s="778" t="s">
+      <c r="W2" s="777" t="s">
         <v>164</v>
       </c>
-      <c r="X2" s="778"/>
-      <c r="Y2" s="778" t="s">
+      <c r="X2" s="777"/>
+      <c r="Y2" s="777" t="s">
         <v>165</v>
       </c>
-      <c r="Z2" s="778"/>
-      <c r="AA2" s="778" t="s">
+      <c r="Z2" s="777"/>
+      <c r="AA2" s="777" t="s">
         <v>166</v>
       </c>
-      <c r="AB2" s="779"/>
-      <c r="AC2" s="776"/>
+      <c r="AB2" s="778"/>
+      <c r="AC2" s="775"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">

</xml_diff>